<commit_message>
Modifs légères de l'Excel
</commit_message>
<xml_diff>
--- a/Planning d'intervention Maintenance CENSURE POUR TESTS.xlsx
+++ b/Planning d'intervention Maintenance CENSURE POUR TESTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1 Dossiers de Nicolas\Etudes EPF\Swish\Code\BotMail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37109655-2E00-4BCC-AAD0-ED85958CB9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57B2CCE-E8C8-41CA-9B37-E5CECD356323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="3ObO7lhbQChKT/Xtw/BLX4lNVq3Cq/6ocFooM4xCcLvSYtChDMF3f+oZspex3tZgOhs11Rh4Nr9DG6JRfkN4cg==" workbookSaltValue="lNSrrGt5psh5kPE8rpctDg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
@@ -1906,29 +1906,34 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W5" sqref="W5:W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24" style="86" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="86" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="86" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="86" customWidth="1"/>
     <col min="3" max="3" width="19.88671875" style="86" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="86" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" style="86" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="86" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" style="86" customWidth="1"/>
-    <col min="8" max="8" width="18" style="86" customWidth="1"/>
-    <col min="9" max="9" width="40.109375" style="86" customWidth="1"/>
-    <col min="10" max="12" width="24.6640625" style="86" customWidth="1"/>
-    <col min="13" max="14" width="24.6640625" style="87" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" style="88" customWidth="1"/>
-    <col min="16" max="17" width="21.33203125" style="89" customWidth="1"/>
-    <col min="18" max="18" width="20.44140625" style="90" customWidth="1"/>
-    <col min="19" max="20" width="20.44140625" style="91" customWidth="1"/>
-    <col min="21" max="21" width="20.88671875" style="92" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="86" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="86" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="86" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" style="86" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="86" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" style="86" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" style="86" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="86" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="86" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="87" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" style="87" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="88" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" style="89" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" style="89" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" style="90" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" style="91" customWidth="1"/>
+    <col min="20" max="20" width="9.77734375" style="91" customWidth="1"/>
+    <col min="21" max="21" width="11.77734375" style="92" customWidth="1"/>
     <col min="22" max="22" width="2.44140625" style="93" customWidth="1"/>
     <col min="23" max="16384" width="11.5546875" style="86"/>
   </cols>
@@ -8952,18 +8957,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8985,18 +8990,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC99D9B8-395A-430E-937C-0EA8E9C71B29}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>